<commit_message>
Added a few logos
</commit_message>
<xml_diff>
--- a/src/places.xlsx
+++ b/src/places.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky Ly\Documents\GitHub\foods-react\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2E4391-99F3-4716-A3D4-474E2FB5EDBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9173C14-32B9-4E9E-8221-DB56922FD135}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="360" windowWidth="21600" windowHeight="15105" xr2:uid="{BF75D567-C03D-4A0E-B5AF-1E6B3567BF9A}"/>
+    <workbookView xWindow="7680" yWindow="0" windowWidth="21600" windowHeight="15105" xr2:uid="{BF75D567-C03D-4A0E-B5AF-1E6B3567BF9A}"/>
   </bookViews>
   <sheets>
     <sheet name="places" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="205">
   <si>
     <t>name</t>
   </si>
@@ -628,6 +628,27 @@
   </si>
   <si>
     <t>Barbecue</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>168-sushi</t>
+  </si>
+  <si>
+    <t>bang-bang</t>
+  </si>
+  <si>
+    <t>banh-mi-boys</t>
+  </si>
+  <si>
+    <t>beavertails</t>
+  </si>
+  <si>
+    <t>boba-boy</t>
+  </si>
+  <si>
+    <t>blaze-pizza</t>
   </si>
 </sst>
 </file>
@@ -979,11 +1000,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A2263A-B294-420A-BF92-275A13F5404B}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,9 +1015,10 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -1021,8 +1043,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1047,8 +1072,11 @@
       <c r="H2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1073,8 +1101,11 @@
       <c r="H3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1099,8 +1130,11 @@
       <c r="H4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1125,8 +1159,11 @@
       <c r="H5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1151,8 +1188,11 @@
       <c r="H6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1177,8 +1217,11 @@
       <c r="H7" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1203,8 +1246,11 @@
       <c r="H8" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1229,8 +1275,11 @@
       <c r="H9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1255,8 +1304,11 @@
       <c r="H10" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1281,8 +1333,11 @@
       <c r="H11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1307,8 +1362,11 @@
       <c r="H12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1333,8 +1391,11 @@
       <c r="H13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1359,8 +1420,11 @@
       <c r="H14" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1385,8 +1449,11 @@
       <c r="H15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1411,8 +1478,11 @@
       <c r="H16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1437,8 +1507,11 @@
       <c r="H17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1463,8 +1536,11 @@
       <c r="H18" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1489,8 +1565,11 @@
       <c r="H19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1515,8 +1594,11 @@
       <c r="H20" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1541,8 +1623,11 @@
       <c r="H21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1567,8 +1652,11 @@
       <c r="H22" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1593,8 +1681,11 @@
       <c r="H23" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1619,8 +1710,11 @@
       <c r="H24" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1645,8 +1739,11 @@
       <c r="H25" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1671,8 +1768,11 @@
       <c r="H26" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1697,8 +1797,11 @@
       <c r="H27" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1723,8 +1826,11 @@
       <c r="H28" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1749,8 +1855,11 @@
       <c r="H29" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1775,8 +1884,11 @@
       <c r="H30" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1801,8 +1913,11 @@
       <c r="H31" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1827,8 +1942,11 @@
       <c r="H32" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1853,8 +1971,11 @@
       <c r="H33" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1879,8 +2000,11 @@
       <c r="H34" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1905,8 +2029,11 @@
       <c r="H35" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1931,8 +2058,11 @@
       <c r="H36" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1957,8 +2087,11 @@
       <c r="H37" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1983,8 +2116,11 @@
       <c r="H38" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2009,8 +2145,11 @@
       <c r="H39" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2035,8 +2174,11 @@
       <c r="H40" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2061,8 +2203,11 @@
       <c r="H41" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2087,8 +2232,11 @@
       <c r="H42" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2113,8 +2261,11 @@
       <c r="H43" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2139,8 +2290,11 @@
       <c r="H44" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2165,8 +2319,11 @@
       <c r="H45" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2191,8 +2348,11 @@
       <c r="H46" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2217,8 +2377,11 @@
       <c r="H47" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2243,8 +2406,11 @@
       <c r="H48" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2269,8 +2435,11 @@
       <c r="H49" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2295,8 +2464,11 @@
       <c r="H50" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2321,8 +2493,11 @@
       <c r="H51" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2347,8 +2522,11 @@
       <c r="H52" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2373,8 +2551,11 @@
       <c r="H53" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2399,8 +2580,11 @@
       <c r="H54" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2425,8 +2609,11 @@
       <c r="H55" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2451,8 +2638,11 @@
       <c r="H56" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2477,8 +2667,11 @@
       <c r="H57" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2503,8 +2696,11 @@
       <c r="H58" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2529,8 +2725,11 @@
       <c r="H59" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2555,8 +2754,11 @@
       <c r="H60" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2581,8 +2783,11 @@
       <c r="H61" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2607,8 +2812,11 @@
       <c r="H62" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2632,6 +2840,9 @@
       </c>
       <c r="H63" t="s">
         <v>181</v>
+      </c>
+      <c r="I63" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more locations to places
</commit_message>
<xml_diff>
--- a/src/places.xlsx
+++ b/src/places.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky Ly\Documents\GitHub\foods-react\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E340F232-C141-49C5-B892-DE3EC2A4D37E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2011EE-B70C-444D-AF57-2BB7C29D10A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="0" windowWidth="21600" windowHeight="15105" xr2:uid="{BF75D567-C03D-4A0E-B5AF-1E6B3567BF9A}"/>
+    <workbookView xWindow="7305" yWindow="60" windowWidth="21600" windowHeight="15105" xr2:uid="{BF75D567-C03D-4A0E-B5AF-1E6B3567BF9A}"/>
   </bookViews>
   <sheets>
     <sheet name="places" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="264">
   <si>
     <t>name</t>
   </si>
@@ -561,12 +561,6 @@
     <t>M5E 1B4</t>
   </si>
   <si>
-    <t>335 Bloor St W</t>
-  </si>
-  <si>
-    <t>M5S 1W7</t>
-  </si>
-  <si>
     <t>106-3623 Highway 7</t>
   </si>
   <si>
@@ -739,6 +733,99 @@
   </si>
   <si>
     <t>machi-machi</t>
+  </si>
+  <si>
+    <t>100-7100 Woodbine Ave</t>
+  </si>
+  <si>
+    <t>L3R 5J2</t>
+  </si>
+  <si>
+    <t>A02-4559 Hurontario St</t>
+  </si>
+  <si>
+    <t>L4Z 3L9</t>
+  </si>
+  <si>
+    <t>399 Yonge St</t>
+  </si>
+  <si>
+    <t>M5B 1S9</t>
+  </si>
+  <si>
+    <t>A11-357 Bremner Blvd</t>
+  </si>
+  <si>
+    <t>M5V 3V4</t>
+  </si>
+  <si>
+    <t>Chop Steakhouse &amp; Bar</t>
+  </si>
+  <si>
+    <t>Steak House</t>
+  </si>
+  <si>
+    <t>41 Colossus Dr</t>
+  </si>
+  <si>
+    <t>L4L 9J8</t>
+  </si>
+  <si>
+    <t>801 Dixon Rd</t>
+  </si>
+  <si>
+    <t>M9W 1J5</t>
+  </si>
+  <si>
+    <t>2001 Argentia Rd</t>
+  </si>
+  <si>
+    <t>L5N 2L3</t>
+  </si>
+  <si>
+    <t>14-5 Northtown Way</t>
+  </si>
+  <si>
+    <t>M2N 7A1</t>
+  </si>
+  <si>
+    <t>105 Queens Quay W</t>
+  </si>
+  <si>
+    <t>M5J 2H2</t>
+  </si>
+  <si>
+    <t>4447 Sheppard Ave E</t>
+  </si>
+  <si>
+    <t>M1S 1V3</t>
+  </si>
+  <si>
+    <t>257 Dundas St E</t>
+  </si>
+  <si>
+    <t>L5A 1W8</t>
+  </si>
+  <si>
+    <t>D108-3278 Midland Ave</t>
+  </si>
+  <si>
+    <t>M1V 0C9</t>
+  </si>
+  <si>
+    <t>105-3985 Highway 7</t>
+  </si>
+  <si>
+    <t>L3R 2A2</t>
+  </si>
+  <si>
+    <t>9 Spring Garden Ave</t>
+  </si>
+  <si>
+    <t>M2N 3G1</t>
+  </si>
+  <si>
+    <t>chop-steakhouse</t>
   </si>
 </sst>
 </file>
@@ -791,6 +878,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{65E5852A-A142-42FA-96C2-B7830030C0E3}" name="Table3" displayName="Table3" ref="A1:I76" totalsRowShown="0">
+  <autoFilter ref="A1:I76" xr:uid="{D3BB4A97-62D8-4845-81F5-B03DCC1825F2}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{984BF25E-1C06-427F-AE7F-EB2F54D4B12E}" name="id">
+      <calculatedColumnFormula>ROW(A1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{46AA7E6B-F4CB-4C00-B564-E3FACB6A9989}" name="name"/>
+    <tableColumn id="3" xr3:uid="{6E143A87-813C-4397-9FEF-0D9C2B3B7F48}" name="category"/>
+    <tableColumn id="4" xr3:uid="{F1FC3BCB-5C9E-404E-81BD-4AD5331A49B3}" name="sub_category"/>
+    <tableColumn id="5" xr3:uid="{2FFD123B-F956-4A4E-9F63-1B6EADDB6911}" name="address"/>
+    <tableColumn id="6" xr3:uid="{36FF64D8-5D55-4235-8A25-00235966B71B}" name="city"/>
+    <tableColumn id="7" xr3:uid="{0C3B96F8-9F04-4462-B11F-8C970D1D6C5A}" name="province"/>
+    <tableColumn id="8" xr3:uid="{63BBFBF7-BCDF-4011-8157-3EDF30783542}" name="postal"/>
+    <tableColumn id="9" xr3:uid="{82DE4C33-160B-46EE-8D62-24080E6A237B}" name="logo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1090,20 +1197,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A2263A-B294-420A-BF92-275A13F5404B}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1134,11 +1242,12 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
+        <f>ROW(A1)</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1163,11 +1272,12 @@
         <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f t="shared" ref="A3:A75" si="0">ROW(A2)</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1192,15 +1302,16 @@
         <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
         <v>134</v>
@@ -1221,11 +1332,12 @@
         <v>163</v>
       </c>
       <c r="I4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1250,11 +1362,12 @@
         <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1279,24 +1392,25 @@
         <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -1305,14 +1419,15 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>150</v>
+        <v>238</v>
       </c>
       <c r="I7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1322,10 +1437,10 @@
         <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -1334,27 +1449,28 @@
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>183</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>182</v>
       </c>
       <c r="E9" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -1363,56 +1479,58 @@
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="I9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
+        <f>ROW(A10)</f>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>239</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -1421,143 +1539,148 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>80</v>
+        <v>240</v>
       </c>
       <c r="I11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
+        <f>ROW(A11)</f>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="I12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="I13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>113</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
@@ -1566,27 +1689,28 @@
         <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="I16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
@@ -1595,27 +1719,28 @@
         <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>38</v>
+        <v>118</v>
       </c>
       <c r="I17" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>183</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
@@ -1624,143 +1749,148 @@
         <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="I18" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>171</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
       </c>
       <c r="H19" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="I19" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
+        <f>ROW(A19)</f>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>241</v>
       </c>
       <c r="C20" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>242</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>243</v>
       </c>
       <c r="F20" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
         <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>101</v>
+        <v>244</v>
       </c>
       <c r="I20" t="s">
-        <v>205</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
+        <f>ROW(A20)</f>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>241</v>
       </c>
       <c r="C21" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>242</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>245</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>246</v>
       </c>
       <c r="I21" t="s">
-        <v>206</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
+        <f>ROW(A21)</f>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="C22" t="s">
-        <v>194</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>242</v>
       </c>
       <c r="E22" t="s">
-        <v>164</v>
+        <v>247</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>165</v>
+        <v>248</v>
       </c>
       <c r="I22" t="s">
-        <v>208</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
+        <f>ROW(A22)</f>
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="C23" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
@@ -1769,56 +1899,58 @@
         <v>11</v>
       </c>
       <c r="H23" t="s">
-        <v>167</v>
+        <v>95</v>
       </c>
       <c r="I23" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="C24" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="G24" t="s">
         <v>11</v>
       </c>
       <c r="H24" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="I24" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="C25" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s">
         <v>100</v>
@@ -1827,288 +1959,298 @@
         <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="I25" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
         <v>11</v>
       </c>
       <c r="H26" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="I26" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
+        <f>ROW(A26)</f>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>249</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
       </c>
       <c r="H27" t="s">
-        <v>89</v>
+        <v>250</v>
       </c>
       <c r="I27" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
+        <f>ROW(A27)</f>
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D28" t="s">
         <v>25</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>251</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
         <v>11</v>
       </c>
       <c r="H28" t="s">
-        <v>108</v>
+        <v>252</v>
       </c>
       <c r="I28" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
+        <f>ROW(A28)</f>
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>205</v>
       </c>
       <c r="C29" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="F29" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="G29" t="s">
         <v>11</v>
       </c>
       <c r="H29" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="I29" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>205</v>
       </c>
       <c r="C30" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>166</v>
       </c>
       <c r="F30" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
       </c>
       <c r="H30" t="s">
-        <v>112</v>
+        <v>167</v>
       </c>
       <c r="I30" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>212</v>
+        <v>133</v>
       </c>
       <c r="C31" t="s">
-        <v>194</v>
+        <v>134</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G31" t="s">
         <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="I31" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>212</v>
+        <v>133</v>
       </c>
       <c r="C32" t="s">
-        <v>194</v>
+        <v>134</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="G32" t="s">
         <v>11</v>
       </c>
       <c r="H32" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="I32" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>185</v>
+        <v>84</v>
       </c>
       <c r="E33" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="G33" t="s">
         <v>11</v>
       </c>
       <c r="H33" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="I33" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="E34" t="s">
-        <v>191</v>
+        <v>88</v>
       </c>
       <c r="F34" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="G34" t="s">
         <v>11</v>
       </c>
       <c r="H34" t="s">
-        <v>192</v>
+        <v>89</v>
       </c>
       <c r="I34" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="D35" t="s">
-        <v>193</v>
+        <v>25</v>
       </c>
       <c r="E35" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="F35" t="s">
         <v>10</v>
@@ -2117,27 +2259,28 @@
         <v>11</v>
       </c>
       <c r="H35" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="I35" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="D36" t="s">
-        <v>193</v>
+        <v>25</v>
       </c>
       <c r="E36" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="F36" t="s">
         <v>71</v>
@@ -2146,56 +2289,58 @@
         <v>11</v>
       </c>
       <c r="H36" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="I36" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="F37" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="G37" t="s">
         <v>11</v>
       </c>
       <c r="H37" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
       <c r="I37" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>210</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>192</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="F38" t="s">
         <v>14</v>
@@ -2204,85 +2349,88 @@
         <v>11</v>
       </c>
       <c r="H38" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
       <c r="I38" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>210</v>
       </c>
       <c r="C39" t="s">
-        <v>134</v>
+        <v>192</v>
       </c>
       <c r="D39" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>22</v>
+        <v>235</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G39" t="s">
         <v>11</v>
       </c>
       <c r="H39" t="s">
-        <v>23</v>
+        <v>236</v>
       </c>
       <c r="I39" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="F40" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="G40" t="s">
         <v>11</v>
       </c>
       <c r="H40" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="I40" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="C41" t="s">
-        <v>194</v>
+        <v>134</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="E41" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
       <c r="F41" t="s">
         <v>14</v>
@@ -2291,288 +2439,298 @@
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>49</v>
+        <v>141</v>
       </c>
       <c r="I41" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>188</v>
       </c>
       <c r="C42" t="s">
-        <v>194</v>
+        <v>72</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>51</v>
+        <v>189</v>
       </c>
       <c r="F42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G42" t="s">
         <v>11</v>
       </c>
       <c r="H42" t="s">
-        <v>53</v>
+        <v>190</v>
       </c>
       <c r="I42" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>72</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
       <c r="E43" t="s">
-        <v>155</v>
+        <v>73</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G43" t="s">
         <v>11</v>
       </c>
       <c r="H43" t="s">
-        <v>156</v>
+        <v>74</v>
       </c>
       <c r="I43" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>72</v>
       </c>
       <c r="D44" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
       <c r="E44" t="s">
-        <v>157</v>
+        <v>75</v>
       </c>
       <c r="F44" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="G44" t="s">
         <v>11</v>
       </c>
       <c r="H44" t="s">
-        <v>158</v>
+        <v>76</v>
       </c>
       <c r="I44" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E45" t="s">
-        <v>130</v>
+        <v>17</v>
       </c>
       <c r="F45" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G45" t="s">
         <v>11</v>
       </c>
       <c r="H45" t="s">
-        <v>131</v>
+        <v>19</v>
       </c>
       <c r="I45" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
+        <f>ROW(A45)</f>
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>132</v>
+        <v>253</v>
       </c>
       <c r="F46" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="G46" t="s">
         <v>11</v>
       </c>
       <c r="H46" t="s">
-        <v>98</v>
+        <v>254</v>
       </c>
       <c r="I46" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
+        <f>ROW(A46)</f>
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="F47" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G47" t="s">
         <v>11</v>
       </c>
       <c r="H47" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="I47" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>187</v>
+        <v>20</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E48" t="s">
-        <v>188</v>
+        <v>22</v>
       </c>
       <c r="F48" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="G48" t="s">
         <v>11</v>
       </c>
       <c r="H48" t="s">
-        <v>189</v>
+        <v>23</v>
       </c>
       <c r="I48" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>168</v>
       </c>
       <c r="C49" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="D49" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="F49" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G49" t="s">
         <v>11</v>
       </c>
       <c r="H49" t="s">
-        <v>92</v>
+        <v>170</v>
       </c>
       <c r="I49" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
+        <f>ROW(A49)</f>
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>231</v>
+        <v>168</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>192</v>
       </c>
       <c r="D50" t="s">
-        <v>186</v>
+        <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>60</v>
+        <v>255</v>
       </c>
       <c r="F50" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G50" t="s">
         <v>11</v>
       </c>
       <c r="H50" t="s">
-        <v>61</v>
+        <v>256</v>
       </c>
       <c r="I50" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
+        <f>ROW(A50)</f>
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>231</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>46</v>
+        <v>192</v>
       </c>
       <c r="D51" t="s">
-        <v>186</v>
+        <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F51" t="s">
         <v>14</v>
@@ -2581,362 +2739,767 @@
         <v>11</v>
       </c>
       <c r="H51" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="I51" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>192</v>
       </c>
       <c r="D52" t="s">
-        <v>184</v>
+        <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>160</v>
+        <v>51</v>
       </c>
       <c r="F52" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="G52" t="s">
         <v>11</v>
       </c>
       <c r="H52" t="s">
-        <v>161</v>
+        <v>53</v>
       </c>
       <c r="I52" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="C53" t="s">
-        <v>32</v>
+        <v>134</v>
       </c>
       <c r="D53" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="E53" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="F53" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="G53" t="s">
         <v>11</v>
       </c>
       <c r="H53" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="I53" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C54" t="s">
         <v>134</v>
       </c>
       <c r="D54" t="s">
-        <v>21</v>
+        <v>154</v>
       </c>
       <c r="E54" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="F54" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="G54" t="s">
         <v>11</v>
       </c>
       <c r="H54" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="I54" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="D55" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E55" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="F55" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="G55" t="s">
         <v>11</v>
       </c>
       <c r="H55" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="I55" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="C56" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D56" t="s">
         <v>25</v>
       </c>
       <c r="E56" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="F56" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="G56" t="s">
         <v>11</v>
       </c>
       <c r="H56" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I56" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D57" t="s">
         <v>25</v>
       </c>
       <c r="E57" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="F57" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G57" t="s">
         <v>11</v>
       </c>
       <c r="H57" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="I57" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
+        <f>ROW(A57)</f>
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D58" t="s">
         <v>25</v>
       </c>
       <c r="E58" t="s">
-        <v>29</v>
+        <v>257</v>
       </c>
       <c r="F58" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="G58" t="s">
         <v>11</v>
       </c>
       <c r="H58" t="s">
-        <v>30</v>
+        <v>258</v>
       </c>
       <c r="I58" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
+        <f>ROW(A58)</f>
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="D59" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="E59" t="s">
-        <v>66</v>
+        <v>259</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="G59" t="s">
         <v>11</v>
       </c>
       <c r="H59" t="s">
-        <v>67</v>
+        <v>260</v>
       </c>
       <c r="I59" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
+        <f>ROW(A59)</f>
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="C60" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>33</v>
+        <v>261</v>
       </c>
       <c r="F60" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G60" t="s">
         <v>11</v>
       </c>
       <c r="H60" t="s">
-        <v>19</v>
+        <v>262</v>
       </c>
       <c r="I60" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
+        <f>ROW(A60)</f>
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>185</v>
       </c>
       <c r="C61" t="s">
-        <v>183</v>
+        <v>72</v>
       </c>
       <c r="D61" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="F61" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="G61" t="s">
         <v>11</v>
       </c>
       <c r="H61" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="I61" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="C62" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D62" t="s">
         <v>25</v>
       </c>
       <c r="E62" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="F62" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G62" t="s">
         <v>11</v>
       </c>
       <c r="H62" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="I62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>229</v>
       </c>
       <c r="C63" t="s">
-        <v>183</v>
+        <v>46</v>
       </c>
       <c r="D63" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
       <c r="E63" t="s">
-        <v>177</v>
+        <v>60</v>
       </c>
       <c r="F63" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="G63" t="s">
         <v>11</v>
       </c>
       <c r="H63" t="s">
-        <v>178</v>
+        <v>61</v>
       </c>
       <c r="I63" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>229</v>
+      </c>
+      <c r="C64" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" t="s">
+        <v>184</v>
+      </c>
+      <c r="E64" t="s">
+        <v>62</v>
+      </c>
+      <c r="F64" t="s">
+        <v>14</v>
+      </c>
+      <c r="G64" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" t="s">
+        <v>63</v>
+      </c>
+      <c r="I64" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>159</v>
+      </c>
+      <c r="C65" t="s">
+        <v>134</v>
+      </c>
+      <c r="D65" t="s">
+        <v>182</v>
+      </c>
+      <c r="E65" t="s">
+        <v>160</v>
+      </c>
+      <c r="F65" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" t="s">
+        <v>161</v>
+      </c>
+      <c r="I65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>177</v>
+      </c>
+      <c r="C66" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>178</v>
+      </c>
+      <c r="F66" t="s">
+        <v>100</v>
+      </c>
+      <c r="G66" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" t="s">
+        <v>179</v>
+      </c>
+      <c r="I66" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" t="s">
+        <v>134</v>
+      </c>
+      <c r="D67" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" t="s">
+        <v>144</v>
+      </c>
+      <c r="F67" t="s">
+        <v>14</v>
+      </c>
+      <c r="G67" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" t="s">
+        <v>145</v>
+      </c>
+      <c r="I67" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" t="s">
+        <v>134</v>
+      </c>
+      <c r="D68" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" t="s">
+        <v>146</v>
+      </c>
+      <c r="F68" t="s">
+        <v>100</v>
+      </c>
+      <c r="G68" t="s">
+        <v>11</v>
+      </c>
+      <c r="H68" t="s">
+        <v>147</v>
+      </c>
+      <c r="I68" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" t="s">
+        <v>181</v>
+      </c>
+      <c r="D69" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" t="s">
+        <v>102</v>
+      </c>
+      <c r="F69" t="s">
+        <v>10</v>
+      </c>
+      <c r="G69" t="s">
+        <v>11</v>
+      </c>
+      <c r="H69" t="s">
+        <v>103</v>
+      </c>
+      <c r="I69" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70" t="s">
+        <v>181</v>
+      </c>
+      <c r="D70" t="s">
+        <v>25</v>
+      </c>
+      <c r="E70" t="s">
+        <v>104</v>
+      </c>
+      <c r="F70" t="s">
+        <v>14</v>
+      </c>
+      <c r="G70" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" t="s">
+        <v>105</v>
+      </c>
+      <c r="I70" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>28</v>
+      </c>
+      <c r="C71" t="s">
+        <v>181</v>
+      </c>
+      <c r="D71" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" t="s">
+        <v>11</v>
+      </c>
+      <c r="H71" t="s">
+        <v>30</v>
+      </c>
+      <c r="I71" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" t="s">
+        <v>65</v>
+      </c>
+      <c r="E72" t="s">
+        <v>66</v>
+      </c>
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" t="s">
+        <v>11</v>
+      </c>
+      <c r="H72" t="s">
+        <v>67</v>
+      </c>
+      <c r="I72" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>31</v>
+      </c>
+      <c r="C73" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" t="s">
+        <v>33</v>
+      </c>
+      <c r="F73" t="s">
+        <v>18</v>
+      </c>
+      <c r="G73" t="s">
+        <v>11</v>
+      </c>
+      <c r="H73" t="s">
+        <v>19</v>
+      </c>
+      <c r="I73" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" t="s">
+        <v>181</v>
+      </c>
+      <c r="D74" t="s">
+        <v>25</v>
+      </c>
+      <c r="E74" t="s">
+        <v>125</v>
+      </c>
+      <c r="F74" t="s">
+        <v>71</v>
+      </c>
+      <c r="G74" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" t="s">
+        <v>126</v>
+      </c>
+      <c r="I74" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75" t="s">
+        <v>181</v>
+      </c>
+      <c r="D75" t="s">
+        <v>25</v>
+      </c>
+      <c r="E75" t="s">
+        <v>127</v>
+      </c>
+      <c r="F75" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" t="s">
+        <v>11</v>
+      </c>
+      <c r="H75" t="s">
+        <v>128</v>
+      </c>
+      <c r="I75" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f>ROW(A75)</f>
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" t="s">
+        <v>181</v>
+      </c>
+      <c r="D76" t="s">
+        <v>25</v>
+      </c>
+      <c r="E76" t="s">
+        <v>175</v>
+      </c>
+      <c r="F76" t="s">
+        <v>71</v>
+      </c>
+      <c r="G76" t="s">
+        <v>11</v>
+      </c>
+      <c r="H76" t="s">
+        <v>176</v>
+      </c>
+      <c r="I76" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>